<commit_message>
06.07.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/April/Othes/RBM 16 to 31 Mar' by dealer.xlsx
+++ b/April/Othes/RBM 16 to 31 Mar' by dealer.xlsx
@@ -804,10 +804,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -864,7 +865,7 @@
       <c r="F3" s="7"/>
       <c r="G3" s="8"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" hidden="1">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
@@ -887,7 +888,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" hidden="1">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -908,7 +909,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" hidden="1">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -929,7 +930,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" hidden="1">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -950,7 +951,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" hidden="1">
       <c r="A8" s="2" t="s">
         <v>17</v>
       </c>
@@ -973,7 +974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" hidden="1">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -994,7 +995,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" hidden="1">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -1015,7 +1016,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" hidden="1">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" hidden="1">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -1059,7 +1060,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" hidden="1">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -1082,7 +1083,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" hidden="1">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
@@ -1105,7 +1106,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" hidden="1">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" hidden="1">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
@@ -1149,7 +1150,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" hidden="1">
       <c r="A17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1170,7 +1171,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" hidden="1">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1191,7 +1192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" hidden="1">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1214,7 +1215,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" hidden="1">
       <c r="A20" s="2" t="s">
         <v>52</v>
       </c>
@@ -1235,7 +1236,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" hidden="1">
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
@@ -1258,7 +1259,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" hidden="1">
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
@@ -1279,7 +1280,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" hidden="1">
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
@@ -1300,7 +1301,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" hidden="1">
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" hidden="1">
       <c r="A25" s="2" t="s">
         <v>52</v>
       </c>
@@ -1344,7 +1345,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" hidden="1">
       <c r="A26" s="2" t="s">
         <v>52</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" hidden="1">
       <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
@@ -1386,7 +1387,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" hidden="1">
       <c r="A28" s="2" t="s">
         <v>52</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" hidden="1">
       <c r="A29" s="2" t="s">
         <v>52</v>
       </c>
@@ -1430,7 +1431,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" hidden="1">
       <c r="A30" s="2" t="s">
         <v>52</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" hidden="1">
       <c r="A31" s="2" t="s">
         <v>52</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" hidden="1">
       <c r="A32" s="2" t="s">
         <v>70</v>
       </c>
@@ -1495,7 +1496,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" hidden="1">
       <c r="A33" s="2" t="s">
         <v>70</v>
       </c>
@@ -1518,7 +1519,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" hidden="1">
       <c r="A34" s="2" t="s">
         <v>70</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" hidden="1">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" hidden="1">
       <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" hidden="1">
       <c r="A37" s="2" t="s">
         <v>70</v>
       </c>
@@ -1610,7 +1611,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" hidden="1">
       <c r="A38" s="2" t="s">
         <v>70</v>
       </c>
@@ -1633,7 +1634,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" hidden="1">
       <c r="A39" s="2" t="s">
         <v>70</v>
       </c>
@@ -1654,7 +1655,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" hidden="1">
       <c r="A40" s="2" t="s">
         <v>70</v>
       </c>
@@ -1677,7 +1678,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" hidden="1">
       <c r="A41" s="2" t="s">
         <v>70</v>
       </c>
@@ -1700,7 +1701,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" hidden="1">
       <c r="A42" s="2" t="s">
         <v>70</v>
       </c>
@@ -1723,7 +1724,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" hidden="1">
       <c r="A43" s="2" t="s">
         <v>70</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" hidden="1">
       <c r="A44" s="2" t="s">
         <v>70</v>
       </c>
@@ -1767,7 +1768,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" hidden="1">
       <c r="A45" s="2" t="s">
         <v>70</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" hidden="1">
       <c r="A46" s="2" t="s">
         <v>70</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" hidden="1">
       <c r="A47" s="2" t="s">
         <v>70</v>
       </c>
@@ -1836,7 +1837,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" hidden="1">
       <c r="A48" s="2" t="s">
         <v>70</v>
       </c>
@@ -1859,7 +1860,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" hidden="1">
       <c r="A49" s="2" t="s">
         <v>70</v>
       </c>
@@ -2084,7 +2085,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:G58"/>
+  <autoFilter ref="A3:G58">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Tulip-2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>

</xml_diff>